<commit_message>
double % of MUR commercial buildings and recalculate distribution
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Albania_COM.xlsx
+++ b/com_mapping_schemes/mapping_Albania_COM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/Exposure_model_validation/com_mapping_schemes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A3BF2-BEBA-7544-97CC-5D044AEB4A39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1858FA1E-84CC-434B-BA45-16176EF6980C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="19820" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11660" yWindow="640" windowWidth="19820" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -31,61 +31,61 @@
     <t>Hotels</t>
   </si>
   <si>
-    <t>0.2% CR/LDUAL+CDM/HBET:6-/Offices
-0.2% CR/LDUAL+CDM/HBET:6-/SOS/Offices
-18.3% CR/LFINF+CDM/H:1/Offices
-3.3% CR/LFINF+CDM/H:2/Offices
-13.3% CR/LFINF+CDM/HBET:3-5/Offices
-2.8% CR/LFINF+CDM/HBET:3-5/SOS/Offices
-9.4% CR+PC/LWAL+CDM/H:1/Offices
-1.0% CR+PC/LWAL+CDM/H:2/Offices
-1.0% CR+PC/LWAL+CDM/HBET:3-5/Offices
-0.6% CR+PC/LWAL+CDM/HBET:6-/Offices
-17.3% MCF/LWAL+CDL/H:1/Offices
-3.4% MCF/LWAL+CDL/H:2/Offices
-6.0% MCF/LWAL+CDL/HBET:3-5/Offices
-20.7% MUR/LWAL+CDN/H:1/Offices
-2.5% MUR/LWAL+CDN/H:2/Offices
-0.0% CR/LFINF+CDL/HBET:3-5/Offices
-0.0% MUR/LWAL+CDN/HBET:3-5/Offices</t>
-  </si>
-  <si>
     <t>0.0% CR/LDUAL+CDM/HBET:6-/Trade
 0.0% CR/LDUAL+CDM/HBET:6-/SOS/Trade
-26.4% CR/LFINF+CDM/H:1/Trade
-5.0% CR/LFINF+CDM/H:2/Trade
+8.73% CR/LFINF+CDM/H:1/Trade
+1.65% CR/LFINF+CDM/H:2/Trade
 0.0% CR/LFINF+CDM/HBET:3-5/Trade
 0.0% CR/LFINF+CDM/HBET:3-5/SOS/Trade
-4.3% CR+PC/LWAL+CDM/H:1/Trade
-2.7% CR+PC/LWAL+CDM/H:2/Trade
+1.42% CR+PC/LWAL+CDM/H:1/Trade
+0.9% CR+PC/LWAL+CDM/H:2/Trade
 0.0% CR+PC/LWAL+CDM/HBET:3-5/Trade
 0.0% CR+PC/LWAL+CDM/HBET:6-/Trade
 28.8% MCF/LWAL+CDL/H:1/Trade
 3.6% MCF/LWAL+CDL/H:2/Trade
 0.0% MCF/LWAL+CDL/HBET:3-5/Trade
-25.7% MUR/LWAL+CDN/H:1/Trade
+51.4% MUR/LWAL+CDN/H:1/Trade
 3.5% MUR/LWAL+CDN/H:2/Trade
 0.0% CR/LFINF+CDL/HBET:3-5/Trade
 0.0% MUR/LWAL+CDN/HBET:3-5/Trade</t>
   </si>
   <si>
-    <t>0.2% CR/LDUAL+CDM/HBET:6-/Hotels
- 0.2% CR/LDUAL+CDM/HBET:6-/SOS/Hotels
- 18.8% CR/LFINF+CDM/H:1/Hotels
- 3.3% CR/LFINF+CDM/H:2/Hotels
- 7.9% CR/LFINF+CDM/HBET:3-5/Hotels
- 0.6% CR/LFINF+CDM/HBET:3-5/SOS/Hotels
- 4.3% CR+PC/LWAL+CDM/H:1/Hotels
- 1.0% CR+PC/LWAL+CDM/H:2/Hotels
- 1.0% CR+PC/LWAL+CDM/HBET:3-5/Hotels
- 0.6% CR+PC/LWAL+CDM/HBET:6-/Hotels
- 28.9% MCF/LWAL+CDL/H:1/Hotels
- 0.2% MCF/LWAL+CDL/H:2/Hotels
- 3.4% MCF/LWAL+CDL/HBET:3-5/Hotels
- 25.7% MUR/LWAL+CDN/H:1/Hotels
- 1.1% MUR/LWAL+CDN/H:2/Hotels
- 0.4% CR/LFINF+CDL/HBET:3-5/Hotels
- 2.4% MUR/LWAL+CDN/HBET:3-5/Hotels</t>
+    <t>0.0% CR/LDUAL+CDM/HBET:6-/Hotels
+0.0% CR/LDUAL+CDM/HBET:6-/SOS/Hotels
+6.47% CR/LFINF+CDM/H:1/Hotels
+1.14% CR/LFINF+CDM/H:2/Hotels
+2.72% CR/LFINF+CDM/HBET:3-5/Hotels
+0.31% CR/LFINF+CDM/HBET:3-5/SOS/Hotels
+1.48% CR+PC/LWAL+CDM/H:1/Hotels
+0.34% CR+PC/LWAL+CDM/H:2/Hotels
+0.34% CR+PC/LWAL+CDM/HBET:3-5/Hotels
+0.0% CR+PC/LWAL+CDM/HBET:6-/Hotels
+28.9% MCF/LWAL+CDL/H:1/Hotels
+0.0% MCF/LWAL+CDL/H:2/Hotels
+3.4% MCF/LWAL+CDL/HBET:3-5/Hotels
+51.4% MUR/LWAL+CDN/H:1/Hotels
+1.1% MUR/LWAL+CDN/H:2/Hotels
+0.0% CR/LFINF+CDL/HBET:3-5/Hotels
+2.4% MUR/LWAL+CDN/HBET:3-5/Hotels</t>
+  </si>
+  <si>
+    <t>0.12% CR/LDUAL+CDM/HBET:6-/Offices
+0.12% CR/LDUAL+CDM/HBET:6-/SOS/Offices
+10.73% CR/LFINF+CDM/H:1/Offices
+1.94% CR/LFINF+CDM/H:2/Offices
+7.80% CR/LFINF+CDM/HBET:3-5/Offices
+1.64% CR/LFINF+CDM/HBET:3-5/SOS/Offices
+5.52% CR+PC/LWAL+CDM/H:1/Offices
+0.59% CR+PC/LWAL+CDM/H:2/Offices
+0.59% CR+PC/LWAL+CDM/HBET:3-5/Offices
+0.35% CR+PC/LWAL+CDM/HBET:6-/Offices
+17.30% MCF/LWAL+CDL/H:1/Offices
+3.40% MCF/LWAL+CDL/H:2/Offices
+6.00% MCF/LWAL+CDL/HBET:3-5/Offices
+41.40% MUR/LWAL+CDN/H:1/Offices
+2.50% MUR/LWAL+CDN/H:2/Offices
+0.0% CR/LFINF+CDL/HBET:3-5/Offices
+0.0% MUR/LWAL+CDN/HBET:3-5/Offices</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -516,13 +516,13 @@
     </row>
     <row r="2" spans="2:4" ht="259" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>